<commit_message>
correct issue in excel template
</commit_message>
<xml_diff>
--- a/lib/Template A.xlsx
+++ b/lib/Template A.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="23760" windowHeight="6780" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="23760" windowHeight="6780"/>
   </bookViews>
   <sheets>
     <sheet name="PAYROLL" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="78">
   <si>
     <t>Monday</t>
   </si>
@@ -1003,6 +1003,15 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1058,15 +1067,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1138,6 +1138,18 @@
     <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1146,18 +1158,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1494,7 +1494,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1504,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1519,26 +1519,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.6" customHeight="1">
-      <c r="A1" s="132"/>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="140" t="s">
+      <c r="A1" s="135"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="143" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="140"/>
-      <c r="F1" s="128" t="s">
+      <c r="E1" s="143"/>
+      <c r="F1" s="131" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="128"/>
-      <c r="H1" s="129"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="132"/>
       <c r="I1" s="106">
         <v>2016</v>
       </c>
-      <c r="J1" s="130" t="s">
+      <c r="J1" s="133" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="131"/>
-      <c r="L1" s="131"/>
+      <c r="K1" s="134"/>
+      <c r="L1" s="134"/>
       <c r="M1" s="79"/>
       <c r="N1" s="42"/>
       <c r="O1" s="42"/>
@@ -2006,10 +2006,10 @@
     <row r="8" spans="1:21" ht="13.5" thickBot="1">
       <c r="A8" s="111"/>
       <c r="B8" s="113"/>
-      <c r="C8" s="143" t="s">
+      <c r="C8" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="144"/>
+      <c r="D8" s="125"/>
       <c r="E8" s="17">
         <v>10</v>
       </c>
@@ -2167,11 +2167,11 @@
       <c r="G10" s="69"/>
       <c r="H10" s="69"/>
       <c r="I10" s="69"/>
-      <c r="J10" s="127" t="s">
+      <c r="J10" s="130" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="127"/>
-      <c r="L10" s="127"/>
+      <c r="K10" s="130"/>
+      <c r="L10" s="130"/>
       <c r="M10" s="69"/>
       <c r="N10" s="42"/>
       <c r="O10" s="42"/>
@@ -2233,11 +2233,15 @@
       <c r="Q11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="R11" s="12"/>
+      <c r="R11" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="S11" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="T11" s="12"/>
+        <v>76</v>
+      </c>
+      <c r="T11" s="12" t="s">
+        <v>77</v>
+      </c>
       <c r="U11" s="13" t="s">
         <v>10</v>
       </c>
@@ -2633,12 +2637,12 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="13.5" thickBot="1">
-      <c r="A17" s="134"/>
-      <c r="B17" s="135"/>
-      <c r="C17" s="145" t="s">
+      <c r="A17" s="137"/>
+      <c r="B17" s="138"/>
+      <c r="C17" s="124" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="144"/>
+      <c r="D17" s="125"/>
       <c r="E17" s="17">
         <v>10</v>
       </c>
@@ -2708,8 +2712,8 @@
       </c>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="136"/>
-      <c r="B18" s="137"/>
+      <c r="A18" s="139"/>
+      <c r="B18" s="140"/>
       <c r="C18" s="94">
         <f>SUM(C12:C17)</f>
         <v>0</v>
@@ -2787,8 +2791,8 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A19" s="138"/>
-      <c r="B19" s="139"/>
+      <c r="A19" s="141"/>
+      <c r="B19" s="142"/>
       <c r="C19" s="69"/>
       <c r="D19" s="69"/>
       <c r="E19" s="69"/>
@@ -2796,11 +2800,11 @@
       <c r="G19" s="69"/>
       <c r="H19" s="69"/>
       <c r="I19" s="69"/>
-      <c r="J19" s="127" t="s">
+      <c r="J19" s="130" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="127"/>
-      <c r="L19" s="127"/>
+      <c r="K19" s="130"/>
+      <c r="L19" s="130"/>
       <c r="M19" s="69"/>
       <c r="N19" s="42"/>
       <c r="O19" s="42"/>
@@ -2862,11 +2866,15 @@
       <c r="Q20" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="R20" s="12"/>
+      <c r="R20" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="S20" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="T20" s="12"/>
+        <v>76</v>
+      </c>
+      <c r="T20" s="12" t="s">
+        <v>77</v>
+      </c>
       <c r="U20" s="13" t="s">
         <v>10</v>
       </c>
@@ -3264,10 +3272,10 @@
     <row r="26" spans="1:21" ht="13.5" thickBot="1">
       <c r="A26" s="113"/>
       <c r="B26" s="118"/>
-      <c r="C26" s="145" t="s">
+      <c r="C26" s="124" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="144"/>
+      <c r="D26" s="125"/>
       <c r="E26" s="17">
         <v>10</v>
       </c>
@@ -3425,11 +3433,11 @@
       <c r="G28" s="69"/>
       <c r="H28" s="69"/>
       <c r="I28" s="69"/>
-      <c r="J28" s="127" t="s">
+      <c r="J28" s="130" t="s">
         <v>38</v>
       </c>
-      <c r="K28" s="127"/>
-      <c r="L28" s="127"/>
+      <c r="K28" s="130"/>
+      <c r="L28" s="130"/>
       <c r="M28" s="69"/>
       <c r="N28" s="42"/>
       <c r="O28" s="42"/>
@@ -3491,11 +3499,15 @@
       <c r="Q29" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="R29" s="12"/>
+      <c r="R29" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="S29" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="T29" s="12"/>
+        <v>76</v>
+      </c>
+      <c r="T29" s="12" t="s">
+        <v>77</v>
+      </c>
       <c r="U29" s="13" t="s">
         <v>10</v>
       </c>
@@ -3891,12 +3903,12 @@
       </c>
     </row>
     <row r="35" spans="1:21" ht="13.5" thickBot="1">
-      <c r="A35" s="134"/>
-      <c r="B35" s="135"/>
-      <c r="C35" s="145" t="s">
+      <c r="A35" s="137"/>
+      <c r="B35" s="138"/>
+      <c r="C35" s="124" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="144"/>
+      <c r="D35" s="125"/>
       <c r="E35" s="17">
         <v>10</v>
       </c>
@@ -3966,8 +3978,8 @@
       </c>
     </row>
     <row r="36" spans="1:21">
-      <c r="A36" s="136"/>
-      <c r="B36" s="137"/>
+      <c r="A36" s="139"/>
+      <c r="B36" s="140"/>
       <c r="C36" s="94">
         <f>SUM(C30:C35)</f>
         <v>0</v>
@@ -4045,8 +4057,8 @@
       </c>
     </row>
     <row r="37" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A37" s="138"/>
-      <c r="B37" s="139"/>
+      <c r="A37" s="141"/>
+      <c r="B37" s="142"/>
       <c r="C37" s="69"/>
       <c r="D37" s="69"/>
       <c r="E37" s="69"/>
@@ -4054,11 +4066,11 @@
       <c r="G37" s="69"/>
       <c r="H37" s="69"/>
       <c r="I37" s="69"/>
-      <c r="J37" s="127" t="s">
+      <c r="J37" s="130" t="s">
         <v>39</v>
       </c>
-      <c r="K37" s="127"/>
-      <c r="L37" s="127"/>
+      <c r="K37" s="130"/>
+      <c r="L37" s="130"/>
       <c r="M37" s="69"/>
       <c r="N37" s="42"/>
       <c r="O37" s="42"/>
@@ -4120,11 +4132,15 @@
       <c r="Q38" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="R38" s="12"/>
+      <c r="R38" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="S38" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="T38" s="12"/>
+        <v>76</v>
+      </c>
+      <c r="T38" s="12" t="s">
+        <v>77</v>
+      </c>
       <c r="U38" s="13" t="s">
         <v>10</v>
       </c>
@@ -4520,12 +4536,12 @@
       </c>
     </row>
     <row r="44" spans="1:21" ht="13.5" thickBot="1">
-      <c r="A44" s="133"/>
-      <c r="B44" s="133"/>
-      <c r="C44" s="143" t="s">
+      <c r="A44" s="136"/>
+      <c r="B44" s="136"/>
+      <c r="C44" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="D44" s="144"/>
+      <c r="D44" s="125"/>
       <c r="E44" s="17">
         <v>10</v>
       </c>
@@ -4595,8 +4611,8 @@
       </c>
     </row>
     <row r="45" spans="1:21">
-      <c r="A45" s="133"/>
-      <c r="B45" s="133"/>
+      <c r="A45" s="136"/>
+      <c r="B45" s="136"/>
       <c r="C45" s="94">
         <f>SUM(C39:C44)</f>
         <v>0</v>
@@ -4674,8 +4690,8 @@
       </c>
     </row>
     <row r="46" spans="1:21" ht="16.5" customHeight="1">
-      <c r="A46" s="133"/>
-      <c r="B46" s="133"/>
+      <c r="A46" s="136"/>
+      <c r="B46" s="136"/>
       <c r="C46" s="69"/>
       <c r="D46" s="69"/>
       <c r="E46" s="69"/>
@@ -4683,11 +4699,11 @@
       <c r="G46" s="69"/>
       <c r="H46" s="69"/>
       <c r="I46" s="69"/>
-      <c r="J46" s="127" t="s">
+      <c r="J46" s="130" t="s">
         <v>46</v>
       </c>
-      <c r="K46" s="127"/>
-      <c r="L46" s="127"/>
+      <c r="K46" s="130"/>
+      <c r="L46" s="130"/>
       <c r="M46" s="69"/>
       <c r="N46" s="42"/>
       <c r="O46" s="42"/>
@@ -4698,8 +4714,8 @@
       <c r="T46" s="67"/>
     </row>
     <row r="47" spans="1:21">
-      <c r="A47" s="133"/>
-      <c r="B47" s="133"/>
+      <c r="A47" s="136"/>
+      <c r="B47" s="136"/>
       <c r="C47" s="112" t="s">
         <v>7</v>
       </c>
@@ -4733,9 +4749,9 @@
       </c>
     </row>
     <row r="48" spans="1:21">
-      <c r="A48" s="133"/>
-      <c r="B48" s="133"/>
-      <c r="C48" s="141"/>
+      <c r="A48" s="136"/>
+      <c r="B48" s="136"/>
+      <c r="C48" s="144"/>
       <c r="D48" s="110" t="s">
         <v>47</v>
       </c>
@@ -4763,9 +4779,9 @@
       </c>
     </row>
     <row r="49" spans="1:21">
-      <c r="A49" s="133"/>
-      <c r="B49" s="133"/>
-      <c r="C49" s="142"/>
+      <c r="A49" s="136"/>
+      <c r="B49" s="136"/>
+      <c r="C49" s="145"/>
       <c r="D49" s="110" t="s">
         <v>48</v>
       </c>
@@ -4791,8 +4807,8 @@
       </c>
     </row>
     <row r="50" spans="1:21" ht="13.5" thickBot="1">
-      <c r="A50" s="133"/>
-      <c r="B50" s="133"/>
+      <c r="A50" s="136"/>
+      <c r="B50" s="136"/>
       <c r="C50" s="94">
         <f>SUM(C49:C49)</f>
         <v>0</v>
@@ -4870,12 +4886,12 @@
       </c>
     </row>
     <row r="51" spans="1:21" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A51" s="133"/>
-      <c r="B51" s="133"/>
-      <c r="C51" s="125" t="s">
+      <c r="A51" s="136"/>
+      <c r="B51" s="136"/>
+      <c r="C51" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="126"/>
+      <c r="D51" s="129"/>
       <c r="E51" s="92">
         <f>+E9+E18+E27+E36+E45+E50</f>
         <v>60</v>
@@ -5099,67 +5115,79 @@
       </c>
     </row>
     <row r="56" spans="1:21" ht="12.75" customHeight="1">
-      <c r="D56" s="124" t="str">
+      <c r="D56" s="127" t="str">
         <f>IF(U55 = 0,"CHECKS GOOD","ERROR IN PRINTOUT")</f>
         <v>CHECKS GOOD</v>
       </c>
-      <c r="E56" s="124"/>
-      <c r="F56" s="124"/>
-      <c r="G56" s="124"/>
-      <c r="H56" s="124"/>
-      <c r="I56" s="124"/>
-      <c r="J56" s="124"/>
-      <c r="K56" s="124"/>
-      <c r="L56" s="124"/>
-      <c r="M56" s="124"/>
-      <c r="N56" s="124"/>
-      <c r="O56" s="124"/>
-      <c r="P56" s="124"/>
-      <c r="Q56" s="124"/>
-      <c r="R56" s="124"/>
-      <c r="S56" s="124"/>
-      <c r="T56" s="124"/>
+      <c r="E56" s="127"/>
+      <c r="F56" s="127"/>
+      <c r="G56" s="127"/>
+      <c r="H56" s="127"/>
+      <c r="I56" s="127"/>
+      <c r="J56" s="127"/>
+      <c r="K56" s="127"/>
+      <c r="L56" s="127"/>
+      <c r="M56" s="127"/>
+      <c r="N56" s="127"/>
+      <c r="O56" s="127"/>
+      <c r="P56" s="127"/>
+      <c r="Q56" s="127"/>
+      <c r="R56" s="127"/>
+      <c r="S56" s="127"/>
+      <c r="T56" s="127"/>
     </row>
     <row r="57" spans="1:21" ht="12.75" customHeight="1">
-      <c r="D57" s="124"/>
-      <c r="E57" s="124"/>
-      <c r="F57" s="124"/>
-      <c r="G57" s="124"/>
-      <c r="H57" s="124"/>
-      <c r="I57" s="124"/>
-      <c r="J57" s="124"/>
-      <c r="K57" s="124"/>
-      <c r="L57" s="124"/>
-      <c r="M57" s="124"/>
-      <c r="N57" s="124"/>
-      <c r="O57" s="124"/>
-      <c r="P57" s="124"/>
-      <c r="Q57" s="124"/>
-      <c r="R57" s="124"/>
-      <c r="S57" s="124"/>
-      <c r="T57" s="124"/>
+      <c r="D57" s="127"/>
+      <c r="E57" s="127"/>
+      <c r="F57" s="127"/>
+      <c r="G57" s="127"/>
+      <c r="H57" s="127"/>
+      <c r="I57" s="127"/>
+      <c r="J57" s="127"/>
+      <c r="K57" s="127"/>
+      <c r="L57" s="127"/>
+      <c r="M57" s="127"/>
+      <c r="N57" s="127"/>
+      <c r="O57" s="127"/>
+      <c r="P57" s="127"/>
+      <c r="Q57" s="127"/>
+      <c r="R57" s="127"/>
+      <c r="S57" s="127"/>
+      <c r="T57" s="127"/>
     </row>
     <row r="58" spans="1:21" ht="12.75" customHeight="1">
-      <c r="D58" s="124"/>
-      <c r="E58" s="124"/>
-      <c r="F58" s="124"/>
-      <c r="G58" s="124"/>
-      <c r="H58" s="124"/>
-      <c r="I58" s="124"/>
-      <c r="J58" s="124"/>
-      <c r="K58" s="124"/>
-      <c r="L58" s="124"/>
-      <c r="M58" s="124"/>
-      <c r="N58" s="124"/>
-      <c r="O58" s="124"/>
-      <c r="P58" s="124"/>
-      <c r="Q58" s="124"/>
-      <c r="R58" s="124"/>
-      <c r="S58" s="124"/>
-      <c r="T58" s="124"/>
+      <c r="D58" s="127"/>
+      <c r="E58" s="127"/>
+      <c r="F58" s="127"/>
+      <c r="G58" s="127"/>
+      <c r="H58" s="127"/>
+      <c r="I58" s="127"/>
+      <c r="J58" s="127"/>
+      <c r="K58" s="127"/>
+      <c r="L58" s="127"/>
+      <c r="M58" s="127"/>
+      <c r="N58" s="127"/>
+      <c r="O58" s="127"/>
+      <c r="P58" s="127"/>
+      <c r="Q58" s="127"/>
+      <c r="R58" s="127"/>
+      <c r="S58" s="127"/>
+      <c r="T58" s="127"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A44:B51"/>
+    <mergeCell ref="A35:B37"/>
+    <mergeCell ref="A17:B19"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J28:L28"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C17:D17"/>
@@ -5168,18 +5196,6 @@
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="J37:L37"/>
     <mergeCell ref="J46:L46"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A44:B51"/>
-    <mergeCell ref="A35:B37"/>
-    <mergeCell ref="A17:B19"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C44:D44"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.11" right="0.05" top="0.1" bottom="7.0000000000000007E-2" header="0" footer="0"/>
@@ -7375,7 +7391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A396" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A396" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E413" sqref="E413"/>
     </sheetView>
   </sheetViews>
@@ -15466,12 +15482,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D654:F654"/>
-    <mergeCell ref="D553:F553"/>
-    <mergeCell ref="D501:F501"/>
-    <mergeCell ref="D399:F399"/>
-    <mergeCell ref="D428:F428"/>
-    <mergeCell ref="D452:F452"/>
     <mergeCell ref="D346:F346"/>
     <mergeCell ref="D603:F603"/>
     <mergeCell ref="D250:F250"/>
@@ -15481,6 +15491,12 @@
     <mergeCell ref="D154:F154"/>
     <mergeCell ref="D202:F202"/>
     <mergeCell ref="D103:F103"/>
+    <mergeCell ref="D654:F654"/>
+    <mergeCell ref="D553:F553"/>
+    <mergeCell ref="D501:F501"/>
+    <mergeCell ref="D399:F399"/>
+    <mergeCell ref="D428:F428"/>
+    <mergeCell ref="D452:F452"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15548,22 +15564,22 @@
       <c r="C2" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="173" t="s">
+      <c r="D2" s="169" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="174"/>
-      <c r="F2" s="173" t="s">
+      <c r="E2" s="171"/>
+      <c r="F2" s="169" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="174"/>
-      <c r="H2" s="173" t="s">
+      <c r="G2" s="171"/>
+      <c r="H2" s="169" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="175"/>
-      <c r="J2" s="175"/>
-      <c r="K2" s="175"/>
-      <c r="L2" s="175"/>
-      <c r="M2" s="174"/>
+      <c r="I2" s="170"/>
+      <c r="J2" s="170"/>
+      <c r="K2" s="170"/>
+      <c r="L2" s="170"/>
+      <c r="M2" s="171"/>
       <c r="O2"/>
       <c r="P2"/>
       <c r="Q2"/>
@@ -15786,12 +15802,12 @@
         <v>62</v>
       </c>
       <c r="G8" s="166"/>
-      <c r="H8" s="169"/>
-      <c r="I8" s="170"/>
-      <c r="J8" s="170"/>
-      <c r="K8" s="170"/>
-      <c r="L8" s="170"/>
-      <c r="M8" s="171"/>
+      <c r="H8" s="173"/>
+      <c r="I8" s="174"/>
+      <c r="J8" s="174"/>
+      <c r="K8" s="174"/>
+      <c r="L8" s="174"/>
+      <c r="M8" s="175"/>
       <c r="O8"/>
       <c r="P8"/>
       <c r="Q8"/>
@@ -20191,12 +20207,33 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H7:M7"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="H6:M6"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="H17:M17"/>
@@ -20213,33 +20250,12 @@
     <mergeCell ref="H14:M14"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="H3:M3"/>
-    <mergeCell ref="H4:M4"/>
-    <mergeCell ref="H5:M5"/>
-    <mergeCell ref="H6:M6"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H7:M7"/>
-    <mergeCell ref="H8:M8"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:M16"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>